<commit_message>
ANALISIS DE LA IMAGEN RANA
</commit_message>
<xml_diff>
--- a/lab2/informe/tabla_1.xlsx
+++ b/lab2/informe/tabla_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RICARDO\OneDrive - UNIVERSIDAD INDUSTRIAL DE SANTANDER\Desktop\COMUNICACIONES_2\labcom2_2024_1\lab2\informe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://correouisedu-my.sharepoint.com/personal/ricardo2171774_correo_uis_edu_co/Documents/Desktop/COMUNICACIONES_2/labcom2_2024_1/lab2/informe/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC8E3AE-3371-44C9-A00E-6A7258DA5168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{3FC8E3AE-3371-44C9-A00E-6A7258DA5168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D9AE100-2B29-4D5C-901A-8819258C4679}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9055086E-3C7E-4D51-B2BD-7944A61A0588}"/>
   </bookViews>
@@ -35,8 +35,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={442C1E61-32BC-4A2B-B78B-803E0D9827A0}</author>
+  </authors>
+  <commentList>
+    <comment ref="K4" authorId="0" shapeId="0" xr:uid="{442C1E61-32BC-4A2B-B78B-803E0D9827A0}">
+      <text>
+        <t xml:space="preserve">[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    A medida que tomamos mas muestras por segundo se puede apreciar mas el comportamiento aleatorio del ruido con mas frecuencia y adicional disminuye la potencia y se hace mas continua. </t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sps</t>
   </si>
@@ -60,19 +78,46 @@
   </si>
   <si>
     <t>Rb[bps]</t>
+  </si>
+  <si>
+    <t>INFINITO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSD AMPLITUD </t>
+  </si>
+  <si>
+    <t>SPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIEMPO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUMENTA LA FRECUNCIA DE ALETORIEDAD </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSD </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -95,9 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -113,6 +161,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="RICARDO JAIMES" id="{3925EFA7-B0E5-4333-9167-311C75F5C170}" userId="S::ricardo2171774@correo.uis.edu.co::72169ae8-05b2-48ae-8652-180225ab12d5" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -430,25 +484,37 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="K4" dT="2024-03-05T21:36:13.95" personId="{3925EFA7-B0E5-4333-9167-311C75F5C170}" id="{442C1E61-32BC-4A2B-B78B-803E0D9827A0}">
+    <text xml:space="preserve">A medida que tomamos mas muestras por segundo se puede apreciar mas el comportamiento aleatorio del ruido con mas frecuencia y adicional disminuye la potencia y se hace mas continua. </text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78156C76-9B97-4A63-A7E7-3AA550ED1C0E}">
-  <dimension ref="B3:H10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78156C76-9B97-4A63-A7E7-3AA550ED1C0E}">
+  <dimension ref="B3:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -470,12 +536,21 @@
       <c r="H4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <f>(G5-F5)</f>
         <v>3.1299999999999994E-2</v>
       </c>
@@ -485,23 +560,34 @@
       <c r="E5">
         <v>32000</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5">
         <v>0.40229999999999999</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5">
         <v>0.43359999999999999</v>
       </c>
       <c r="H5">
         <f>1/C5*1000</f>
         <v>31948.881789137384</v>
       </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K5" s="1">
+        <v>3.1300000000000002E-5</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
-        <f t="shared" ref="C6:C9" si="0">(G6-F6)</f>
+      <c r="C6">
+        <f t="shared" ref="C6:C8" si="0">(G6-F6)</f>
         <v>2.7299999999999991E-2</v>
       </c>
       <c r="D6">
@@ -517,15 +603,24 @@
         <v>0.15429999999999999</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H9" si="1">1/C6*1000</f>
+        <f t="shared" ref="H6:H8" si="1">1/C6*1000</f>
         <v>36630.036630036644</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K6" s="1">
+        <v>7.7500000000000003E-6</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>16</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <f t="shared" si="0"/>
         <v>3.1299999999999994E-2</v>
       </c>
@@ -545,14 +640,29 @@
         <f t="shared" si="1"/>
         <v>31948.881789137384</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="K7" s="1">
+        <v>3.8999999999999999E-6</v>
+      </c>
+      <c r="L7">
+        <v>8</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <f t="shared" si="0"/>
         <v>3.1199999999999992E-2</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
       </c>
       <c r="F8">
         <v>7.8200000000000006E-2</v>
@@ -564,14 +674,58 @@
         <f t="shared" si="1"/>
         <v>32051.282051282058</v>
       </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C10" s="1"/>
+      <c r="K8" s="1">
+        <v>1.9599999999999999E-6</v>
+      </c>
+      <c r="L8">
+        <v>16</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>5.9999999999999995E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>3.6000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>2.2000000000000001E-4</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M5:O8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>